<commit_message>
Feat: StageController 정상화 및 기록 저장
</commit_message>
<xml_diff>
--- a/Assets/@Project/Scripts/Data/RawData/LevelDbSheet.xlsx
+++ b/Assets/@Project/Scripts/Data/RawData/LevelDbSheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27612"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5D87BB9-984E-46B7-BFA3-BC6659EE7BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{62EF933A-9ABC-4EA1-AAF0-CAC65B8D9789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
   <si>
     <t>dev_ID</t>
   </si>
@@ -54,12 +54,18 @@
     <t>spawnType3</t>
   </si>
   <si>
+    <t>enemyType</t>
+  </si>
+  <si>
     <t>Minion_Ball</t>
   </si>
   <si>
     <t>None</t>
   </si>
   <si>
+    <t>Minion</t>
+  </si>
+  <si>
     <t>Minion_Spider</t>
   </si>
   <si>
@@ -67,6 +73,9 @@
   </si>
   <si>
     <t>Boss_SkyFire</t>
+  </si>
+  <si>
+    <t>Boss</t>
   </si>
 </sst>
 </file>
@@ -447,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -461,9 +470,10 @@
     <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="6" width="15.125" customWidth="1"/>
     <col min="7" max="7" width="15.625" customWidth="1"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1">
+    <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -485,215 +495,245 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1">
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="3" customFormat="1">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="3" customFormat="1">
+        <v>9</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="3" customFormat="1">
+        <v>9</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="3" customFormat="1">
+        <v>9</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="3" customFormat="1">
+        <v>9</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="3" customFormat="1">
+        <v>12</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="3" customFormat="1">
+        <v>12</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="3" customFormat="1">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -704,23 +744,26 @@
         <v>0</v>
       </c>
       <c r="D11" s="3">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="3" customFormat="1"/>
-    <row r="13" spans="1:7" s="3" customFormat="1"/>
-    <row r="14" spans="1:7" s="3" customFormat="1"/>
-    <row r="15" spans="1:7" s="3" customFormat="1"/>
-    <row r="16" spans="1:7" s="3" customFormat="1"/>
+        <v>9</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="3" customFormat="1"/>
+    <row r="13" spans="1:8" s="3" customFormat="1"/>
+    <row r="14" spans="1:8" s="3" customFormat="1"/>
+    <row r="15" spans="1:8" s="3" customFormat="1"/>
+    <row r="16" spans="1:8" s="3" customFormat="1"/>
     <row r="17" s="3" customFormat="1"/>
     <row r="18" s="3" customFormat="1"/>
     <row r="19" s="3" customFormat="1"/>

</xml_diff>